<commit_message>
fix bug prices dont changew in xlsx for someon artics
</commit_message>
<xml_diff>
--- a/Listas de precios/mayorista/BULON CABEZA HEXAGONAL DISMAY.xlsx
+++ b/Listas de precios/mayorista/BULON CABEZA HEXAGONAL DISMAY.xlsx
@@ -717,7 +717,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="16" t="n">
-        <v>45406</v>
+        <v>45415</v>
       </c>
       <c r="E1" s="3" t="n"/>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="C34" s="14" t="n"/>
       <c r="D34" s="6" t="n">
-        <v>2613.07</v>
+        <v>1358.666</v>
       </c>
     </row>
     <row r="35" ht="18" customHeight="1" s="17">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="C66" s="14" t="n"/>
       <c r="D66" s="6" t="n">
-        <v>4896.86</v>
+        <v>2546.123</v>
       </c>
     </row>
     <row r="67" ht="18" customHeight="1" s="17">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="C67" s="14" t="n"/>
       <c r="D67" s="6" t="n">
-        <v>4940.37</v>
+        <v>2568.745</v>
       </c>
     </row>
     <row r="68" ht="18" customHeight="1" s="17">

</xml_diff>